<commit_message>
Update to ionizing radiations impact categories + correction of few errors in mapping of simapro.
</commit_message>
<xml_diff>
--- a/Data/mappings/ei35/ei_iw_mapping.xlsx
+++ b/Data/mappings/ei35/ei_iw_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\ei35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5564911-519F-4C22-AE98-5F9CAC0901F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95992CD9-68D1-450C-8F90-CCFD7DD6DABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1352</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterate="1" iterateCount="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3759" uniqueCount="1497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3765" uniqueCount="1498">
   <si>
     <t>iw name</t>
   </si>
@@ -4514,6 +4514,9 @@
   </si>
   <si>
     <t>Transformation, to secondary vegetation</t>
+  </si>
+  <si>
+    <t>Curium-alpha</t>
   </si>
 </sst>
 </file>
@@ -4918,9 +4921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1352"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5577,6 +5578,9 @@
       <c r="A61" t="s">
         <v>780</v>
       </c>
+      <c r="B61" t="s">
+        <v>780</v>
+      </c>
       <c r="C61" t="s">
         <v>1480</v>
       </c>
@@ -7859,6 +7863,9 @@
       <c r="A284" t="s">
         <v>880</v>
       </c>
+      <c r="B284" t="s">
+        <v>1497</v>
+      </c>
       <c r="C284" t="s">
         <v>1480</v>
       </c>
@@ -10748,7 +10755,7 @@
         <v>990</v>
       </c>
       <c r="B564" t="s">
-        <v>30</v>
+        <v>560</v>
       </c>
       <c r="C564" t="s">
         <v>1480</v>
@@ -11273,7 +11280,7 @@
         <v>513</v>
       </c>
       <c r="B618" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C618" t="s">
         <v>1480</v>
@@ -15164,8 +15171,14 @@
       <c r="A989" t="s">
         <v>1207</v>
       </c>
+      <c r="B989" t="s">
+        <v>503</v>
+      </c>
       <c r="C989" t="s">
         <v>1480</v>
+      </c>
+      <c r="D989" t="s">
+        <v>1468</v>
       </c>
     </row>
     <row r="990" spans="1:4" x14ac:dyDescent="0.3">
@@ -15323,6 +15336,9 @@
       <c r="A1007" t="s">
         <v>1220</v>
       </c>
+      <c r="B1007" t="s">
+        <v>1220</v>
+      </c>
       <c r="C1007" t="s">
         <v>1480</v>
       </c>
@@ -15895,6 +15911,9 @@
       <c r="A1065" t="s">
         <v>1262</v>
       </c>
+      <c r="B1065" t="s">
+        <v>1262</v>
+      </c>
       <c r="C1065" t="s">
         <v>1480</v>
       </c>
@@ -18578,7 +18597,7 @@
         <v>1445</v>
       </c>
       <c r="B1320" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="C1320" t="s">
         <v>1480</v>
@@ -18682,7 +18701,7 @@
         <v>525</v>
       </c>
       <c r="B1330" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C1330" t="s">
         <v>1480</v>

</xml_diff>

<commit_message>
2.0.1 version. Includes the creation of the footprint version of IW+, update to IPCC2021 AR6 and corrections for land use CFs.
</commit_message>
<xml_diff>
--- a/Data/mappings/ei35/ei_iw_mapping.xlsx
+++ b/Data/mappings/ei35/ei_iw_mapping.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\11max\PycharmProjects\IW_Reborn\Data\mappings\ei35\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95992CD9-68D1-450C-8F90-CCFD7DD6DABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD410246-1856-4207-8F24-D9C55C46CE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4599,9 +4599,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4639,9 +4639,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4674,26 +4674,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4726,26 +4709,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4921,7 +4887,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1352"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1244" workbookViewId="0">
+      <selection activeCell="A1259" sqref="A1259"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -13263,7 +13231,7 @@
         <v>1113</v>
       </c>
       <c r="B807" t="s">
-        <v>1474</v>
+        <v>1138</v>
       </c>
       <c r="C807" t="s">
         <v>1480</v>
@@ -13274,7 +13242,7 @@
         <v>1114</v>
       </c>
       <c r="B808" t="s">
-        <v>1474</v>
+        <v>1138</v>
       </c>
       <c r="C808" t="s">
         <v>1480</v>
@@ -13417,7 +13385,7 @@
         <v>1127</v>
       </c>
       <c r="B821" t="s">
-        <v>1474</v>
+        <v>1138</v>
       </c>
       <c r="C821" t="s">
         <v>1480</v>
@@ -13538,7 +13506,7 @@
         <v>1138</v>
       </c>
       <c r="B832" t="s">
-        <v>1473</v>
+        <v>1138</v>
       </c>
       <c r="C832" t="s">
         <v>1480</v>
@@ -17025,7 +16993,7 @@
         <v>1327</v>
       </c>
       <c r="B1173" t="s">
-        <v>1483</v>
+        <v>1352</v>
       </c>
       <c r="C1173" t="s">
         <v>1480</v>
@@ -17036,7 +17004,7 @@
         <v>1328</v>
       </c>
       <c r="B1174" t="s">
-        <v>1483</v>
+        <v>1352</v>
       </c>
       <c r="C1174" t="s">
         <v>1480</v>
@@ -17179,7 +17147,7 @@
         <v>1341</v>
       </c>
       <c r="B1187" t="s">
-        <v>1483</v>
+        <v>1352</v>
       </c>
       <c r="C1187" t="s">
         <v>1480</v>
@@ -17300,7 +17268,7 @@
         <v>1352</v>
       </c>
       <c r="B1198" t="s">
-        <v>1482</v>
+        <v>1352</v>
       </c>
       <c r="C1198" t="s">
         <v>1480</v>
@@ -17685,7 +17653,7 @@
         <v>1387</v>
       </c>
       <c r="B1233" t="s">
-        <v>1491</v>
+        <v>1412</v>
       </c>
       <c r="C1233" t="s">
         <v>1480</v>
@@ -17696,7 +17664,7 @@
         <v>1388</v>
       </c>
       <c r="B1234" t="s">
-        <v>1491</v>
+        <v>1412</v>
       </c>
       <c r="C1234" t="s">
         <v>1480</v>
@@ -17839,7 +17807,7 @@
         <v>1401</v>
       </c>
       <c r="B1247" t="s">
-        <v>1491</v>
+        <v>1412</v>
       </c>
       <c r="C1247" t="s">
         <v>1480</v>
@@ -17960,7 +17928,7 @@
         <v>1412</v>
       </c>
       <c r="B1258" t="s">
-        <v>1490</v>
+        <v>1412</v>
       </c>
       <c r="C1258" t="s">
         <v>1480</v>

</xml_diff>